<commit_message>
astah fixed -> wrong merge
</commit_message>
<xml_diff>
--- a/Dokumente/Arbeitsaufteilung Termine.xlsx
+++ b/Dokumente/Arbeitsaufteilung Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="0" windowWidth="18540" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="465" yWindow="0" windowWidth="18540" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -344,104 +344,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="95">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -769,24 +774,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -817,7 +822,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -835,7 +840,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -853,7 +858,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -871,7 +876,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -888,7 +893,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -905,7 +910,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -923,7 +928,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -941,7 +946,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -957,7 +962,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -975,7 +980,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -993,7 +998,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1009,7 +1014,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1025,7 +1030,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>41666</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1067,7 @@
         <v>41668</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1077,7 +1082,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1095,7 +1100,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1113,7 +1118,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1129,7 +1134,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1147,7 +1152,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1165,7 +1170,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1181,7 +1186,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1197,7 +1202,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -1213,7 +1218,7 @@
         <v>41682</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>41656</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1249,7 +1254,7 @@
         <v>41656</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1265,7 +1270,7 @@
         <v>41656</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1283,7 +1288,7 @@
         <v>41656</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1301,7 +1306,7 @@
         <v>41656</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1312,7 +1317,7 @@
         <v>41656</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -1328,7 +1333,7 @@
         <v>41689</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
@@ -1344,7 +1349,7 @@
         <v>41692</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1355,7 +1360,7 @@
         <v>41692</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>48</v>
       </c>
@@ -1366,7 +1371,7 @@
         <v>41693</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1392,7 +1397,7 @@
         <v>41693</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1408,7 @@
         <v>41694</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1429,7 +1434,7 @@
         <v>41694</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1460,7 @@
         <v>41695</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>